<commit_message>
added an option to configure the cost function so that it would vary prelims/finals/prelim-finals
</commit_message>
<xml_diff>
--- a/data/schema.xlsx
+++ b/data/schema.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alan.sun/Documents/18-19/ee/eventSelectionOptimization/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF65F1DA-0101-3E4C-90E5-01BADB3688C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="380" yWindow="440" windowWidth="26200" windowHeight="13480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy" sheetId="1" r:id="rId1"/>
+    <sheet name="Scoring" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>FR50m</t>
   </si>
@@ -109,8 +116,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +180,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -219,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,9 +266,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,6 +318,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,14 +511,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,7 +581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -561,13 +619,13 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -582,7 +640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -605,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -629,7 +687,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -641,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -649,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -679,10 +737,10 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -691,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -700,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -714,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -729,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -741,10 +799,10 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -759,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -779,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -794,16 +852,16 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -815,10 +873,10 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -844,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -859,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -877,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -891,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -915,13 +973,13 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -933,10 +991,10 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -944,7 +1002,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -995,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1012,10 +1070,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1024,7 +1082,7 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1036,10 +1094,10 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1054,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1071,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1086,19 +1144,19 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11">
         <v>0</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1107,13 +1165,13 @@
         <v>0</v>
       </c>
       <c r="R11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1124,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1154,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <v>1</v>
@@ -1172,12 +1230,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1207,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1228,7 +1286,786 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C7D3E4-DFCD-9D4F-9EFC-9EED21CAE06B}">
+  <dimension ref="A1:S13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:S13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>13</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>7</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>3.25</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>1.25</v>
+      </c>
+      <c r="S3">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <v>9</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>12</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>2.5</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>4</v>
+      </c>
+      <c r="R4">
+        <v>1.25</v>
+      </c>
+      <c r="S4">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>12</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>1.25</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>13</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <v>12</v>
+      </c>
+      <c r="N8">
+        <v>0.25</v>
+      </c>
+      <c r="O8">
+        <v>1.75</v>
+      </c>
+      <c r="P8">
+        <v>0.25</v>
+      </c>
+      <c r="Q8">
+        <v>0.75</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>3.25</v>
+      </c>
+      <c r="O9">
+        <v>0.5</v>
+      </c>
+      <c r="P9">
+        <v>3.25</v>
+      </c>
+      <c r="Q9">
+        <v>2.75</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>7</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>2.25</v>
+      </c>
+      <c r="R10">
+        <v>2.5</v>
+      </c>
+      <c r="S10">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>16</v>
+      </c>
+      <c r="H11">
+        <v>16</v>
+      </c>
+      <c r="I11">
+        <v>16</v>
+      </c>
+      <c r="J11">
+        <v>16</v>
+      </c>
+      <c r="K11">
+        <v>16</v>
+      </c>
+      <c r="L11">
+        <v>16</v>
+      </c>
+      <c r="M11">
+        <v>16</v>
+      </c>
+      <c r="N11">
+        <v>3.25</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
+      <c r="P11">
+        <v>3.25</v>
+      </c>
+      <c r="Q11">
+        <v>4</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>1.75</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>1.75</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
output time schema in addition to score schema and strategy schema
</commit_message>
<xml_diff>
--- a/data/schema.xlsx
+++ b/data/schema.xlsx
@@ -1,27 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alan.sun/Documents/18-19/ee/eventSelectionOptimization/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF65F1DA-0101-3E4C-90E5-01BADB3688C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="440" windowWidth="26200" windowHeight="13480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy" sheetId="1" r:id="rId1"/>
-    <sheet name="Scoring" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>FR50m</t>
   </si>
@@ -116,8 +109,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,14 +173,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -234,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,27 +251,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -318,24 +285,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -511,21 +460,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +523,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -640,7 +582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -699,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -758,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -817,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -876,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -935,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -994,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1053,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1112,7 +1054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1171,7 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1230,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1278,785 +1220,6 @@
       </c>
       <c r="P13">
         <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C7D3E4-DFCD-9D4F-9EFC-9EED21CAE06B}">
-  <dimension ref="A1:S13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:S13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>16</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>13</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>7</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>3.25</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3">
-        <v>11</v>
-      </c>
-      <c r="K3">
-        <v>9</v>
-      </c>
-      <c r="L3">
-        <v>11</v>
-      </c>
-      <c r="M3">
-        <v>7</v>
-      </c>
-      <c r="N3">
-        <v>3</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>3</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>1.25</v>
-      </c>
-      <c r="S3">
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>16</v>
-      </c>
-      <c r="G4">
-        <v>16</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="J4">
-        <v>7</v>
-      </c>
-      <c r="K4">
-        <v>9</v>
-      </c>
-      <c r="L4">
-        <v>5</v>
-      </c>
-      <c r="M4">
-        <v>12</v>
-      </c>
-      <c r="N4">
-        <v>3</v>
-      </c>
-      <c r="O4">
-        <v>2.5</v>
-      </c>
-      <c r="P4">
-        <v>3</v>
-      </c>
-      <c r="Q4">
-        <v>4</v>
-      </c>
-      <c r="R4">
-        <v>1.25</v>
-      </c>
-      <c r="S4">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>11</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>5</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>16</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>10</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>3</v>
-      </c>
-      <c r="M7">
-        <v>12</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>1.25</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>13</v>
-      </c>
-      <c r="E8">
-        <v>16</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-      <c r="K8">
-        <v>13</v>
-      </c>
-      <c r="L8">
-        <v>7</v>
-      </c>
-      <c r="M8">
-        <v>12</v>
-      </c>
-      <c r="N8">
-        <v>0.25</v>
-      </c>
-      <c r="O8">
-        <v>1.75</v>
-      </c>
-      <c r="P8">
-        <v>0.25</v>
-      </c>
-      <c r="Q8">
-        <v>0.75</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>11</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>3.25</v>
-      </c>
-      <c r="O9">
-        <v>0.5</v>
-      </c>
-      <c r="P9">
-        <v>3.25</v>
-      </c>
-      <c r="Q9">
-        <v>2.75</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>7</v>
-      </c>
-      <c r="F10">
-        <v>9</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>10</v>
-      </c>
-      <c r="J10">
-        <v>7</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>2.25</v>
-      </c>
-      <c r="R10">
-        <v>2.5</v>
-      </c>
-      <c r="S10">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>16</v>
-      </c>
-      <c r="D11">
-        <v>16</v>
-      </c>
-      <c r="E11">
-        <v>16</v>
-      </c>
-      <c r="F11">
-        <v>16</v>
-      </c>
-      <c r="G11">
-        <v>16</v>
-      </c>
-      <c r="H11">
-        <v>16</v>
-      </c>
-      <c r="I11">
-        <v>16</v>
-      </c>
-      <c r="J11">
-        <v>16</v>
-      </c>
-      <c r="K11">
-        <v>16</v>
-      </c>
-      <c r="L11">
-        <v>16</v>
-      </c>
-      <c r="M11">
-        <v>16</v>
-      </c>
-      <c r="N11">
-        <v>3.25</v>
-      </c>
-      <c r="O11">
-        <v>4</v>
-      </c>
-      <c r="P11">
-        <v>3.25</v>
-      </c>
-      <c r="Q11">
-        <v>4</v>
-      </c>
-      <c r="R11">
-        <v>4</v>
-      </c>
-      <c r="S11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>12</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>2</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13">
-        <v>7</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>7</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>9</v>
-      </c>
-      <c r="L13">
-        <v>4</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>1.75</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>1.75</v>
       </c>
       <c r="Q13">
         <v>0</v>

</xml_diff>

<commit_message>
added time series filtration
</commit_message>
<xml_diff>
--- a/data/schema.xlsx
+++ b/data/schema.xlsx
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -561,13 +561,13 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -605,25 +605,25 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -638,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -670,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -679,10 +679,10 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -691,7 +691,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -714,7 +714,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -729,7 +729,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -741,10 +741,10 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -794,16 +794,16 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -841,7 +841,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -859,10 +859,10 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -871,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
         <v>0</v>
@@ -891,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -906,10 +906,10 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -918,10 +918,10 @@
         <v>1</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -933,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -980,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
         <v>1</v>
@@ -1012,7 +1012,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1021,10 +1021,10 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1036,16 +1036,16 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -1077,10 +1077,10 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1098,13 +1098,13 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11">
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
         <v>0</v>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -1219,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
         <v>0</v>

</xml_diff>

<commit_message>
documentation for role of each file
</commit_message>
<xml_diff>
--- a/data/schema.xlsx
+++ b/data/schema.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alansun/Documents/18-19/ee/app/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46726977-32CF-3445-A4AD-75AF9ABCDD96}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23240" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -109,8 +115,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +179,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -219,7 +233,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,9 +265,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,6 +317,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,14 +510,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="16" width="18.83203125" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.1640625" customWidth="1"/>
+    <col min="19" max="19" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,7 +581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -582,7 +640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -641,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -649,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -679,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -700,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -759,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -803,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -818,7 +876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -862,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -877,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -921,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -933,10 +991,10 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -983,10 +1041,10 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -995,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1045,16 +1103,16 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10">
         <v>0</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1062,16 +1120,16 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1080,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1113,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1151,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1172,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1216,10 +1274,10 @@
         <v>1</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
         <v>0</v>

</xml_diff>